<commit_message>
new changes for v1 of flux manuscript
</commit_message>
<xml_diff>
--- a/Meta_Data/Ingalls_Lab_Data/Culture_Meta_Data.xlsx
+++ b/Meta_Data/Ingalls_Lab_Data/Culture_Meta_Data.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/j_sacks/Documents/GitHub/Marine_Betaine_Cycling/Meta_Data/Ingalls_Lab_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048CD5D5-BED7-8F4E-95D6-07F241F8B57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C0DD3C-CE5A-BD4E-8668-400A5BBD635F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15420" yWindow="500" windowWidth="13000" windowHeight="16440" xr2:uid="{2E733B13-9F69-514A-9FE5-836A2034DC6A}"/>
+    <workbookView xWindow="9860" yWindow="3220" windowWidth="18560" windowHeight="16440" xr2:uid="{2E733B13-9F69-514A-9FE5-836A2034DC6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="165">
   <si>
     <t>Organism</t>
   </si>
@@ -528,6 +528,9 @@
   </si>
   <si>
     <t>cells_filt</t>
+  </si>
+  <si>
+    <t>cell_volume_on_filter_uL</t>
   </si>
 </sst>
 </file>
@@ -555,12 +558,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -575,11 +584,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -916,19 +927,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80A0962E-4786-B842-99FB-ABAC8C3D4A32}">
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="99" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="99" workbookViewId="0">
+      <selection activeCell="F121" sqref="F121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.1640625" customWidth="1"/>
     <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="6" max="6" width="24.5" customWidth="1"/>
     <col min="7" max="7" width="15.1640625" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -944,8 +956,11 @@
       <c r="E1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -962,7 +977,7 @@
         <v>4475028000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -979,7 +994,7 @@
         <v>5213700000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -996,7 +1011,7 @@
         <v>4784448000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1013,7 +1028,7 @@
         <v>174627000.00000003</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1030,7 +1045,7 @@
         <v>156178731.80824301</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1047,7 +1062,7 @@
         <v>222528000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1064,7 +1079,7 @@
         <v>283452000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1081,7 +1096,7 @@
         <v>374670000.00000006</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1098,7 +1113,7 @@
         <v>354339999.99999994</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1115,7 +1130,7 @@
         <v>4045536000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1132,7 +1147,7 @@
         <v>4091220000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1149,7 +1164,7 @@
         <v>3661487999.9999995</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1166,7 +1181,7 @@
         <v>3189528000</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1183,7 +1198,7 @@
         <v>3762636000.0000005</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1472,7 +1487,7 @@
         <v>3386280000</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -1489,7 +1504,7 @@
         <v>3313187999.9999995</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1506,7 +1521,7 @@
         <v>3475224000</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -1523,7 +1538,7 @@
         <v>1642140000</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -1540,7 +1555,7 @@
         <v>1896700000</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -1550,8 +1565,11 @@
       <c r="C37" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37">
+        <v>0.11362</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -1561,8 +1579,11 @@
       <c r="C38" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38">
+        <v>0.10396</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -1572,8 +1593,11 @@
       <c r="C39" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39">
+        <v>9.9820000000000006E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -1584,7 +1608,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>43</v>
       </c>
@@ -1595,7 +1619,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -1606,7 +1630,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -1617,7 +1641,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>61</v>
       </c>
@@ -1633,8 +1657,11 @@
       <c r="E44">
         <v>1769468849.8402557</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44">
+        <v>0.31850000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>62</v>
       </c>
@@ -1650,8 +1677,11 @@
       <c r="E45">
         <v>1936571769.8586504</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45">
+        <v>0.34858</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>63</v>
       </c>
@@ -1667,8 +1697,11 @@
       <c r="E46">
         <v>1761162140.5750799</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46">
+        <v>0.31701000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>64</v>
       </c>
@@ -1684,8 +1717,11 @@
       <c r="E47">
         <v>2204716157.2052402</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47">
+        <v>2.20472</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>65</v>
       </c>
@@ -1701,8 +1737,11 @@
       <c r="E48">
         <v>2189278432.9402361</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48">
+        <v>2.1892800000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>66</v>
       </c>
@@ -1718,8 +1757,11 @@
       <c r="E49">
         <v>707997613.83972955</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49">
+        <v>0.70799999999999996</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>67</v>
       </c>
@@ -1735,8 +1777,11 @@
       <c r="E50">
         <v>754840255.59105432</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50">
+        <v>0.75483999999999996</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>68</v>
       </c>
@@ -1752,8 +1797,11 @@
       <c r="E51">
         <v>92781450</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51">
+        <v>3.7112579999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>69</v>
       </c>
@@ -1769,8 +1817,11 @@
       <c r="E52">
         <v>133775795.45454545</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52">
+        <v>5.3510318180000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>70</v>
       </c>
@@ -1786,8 +1837,11 @@
       <c r="E53">
         <v>87888214.285714298</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53">
+        <v>3.5155285709999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>71</v>
       </c>
@@ -1803,8 +1857,11 @@
       <c r="E54">
         <v>2514201714.1718159</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54">
+        <v>0.45255630899999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>72</v>
       </c>
@@ -1820,8 +1877,11 @@
       <c r="E55">
         <v>2708256789.1373801</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55">
+        <v>0.48748622200000002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>73</v>
       </c>
@@ -1837,8 +1897,11 @@
       <c r="E56">
         <v>2594914240.1276422</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56">
+        <v>0.46708456300000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>74</v>
       </c>
@@ -1854,8 +1917,11 @@
       <c r="E57">
         <v>2171574129.3532338</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57">
+        <v>0.39088334299999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>75</v>
       </c>
@@ -1871,8 +1937,11 @@
       <c r="E58">
         <v>1924996996.9969969</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58">
+        <v>0.34649945900000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>76</v>
       </c>
@@ -1888,8 +1957,11 @@
       <c r="E59">
         <v>2194837422.7009773</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59">
+        <v>0.39507073599999998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>77</v>
       </c>
@@ -1905,8 +1977,11 @@
       <c r="E60">
         <v>251553166.06929511</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60">
+        <v>6.2888291999999998E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>78</v>
       </c>
@@ -1922,8 +1997,11 @@
       <c r="E61">
         <v>217620000</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61">
+        <v>5.4405000000000002E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>79</v>
       </c>
@@ -1939,8 +2017,11 @@
       <c r="E62">
         <v>219701953.74800643</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62">
+        <v>5.4925488000000001E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>85</v>
       </c>
@@ -1956,8 +2037,11 @@
       <c r="E63">
         <v>50148540</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63">
+        <v>7.0207955999999996</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>86</v>
       </c>
@@ -1972,6 +2056,9 @@
       </c>
       <c r="E64">
         <v>16325181.818181818</v>
+      </c>
+      <c r="F64">
+        <v>2.2855254550000002</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
@@ -1990,6 +2077,9 @@
       <c r="E65">
         <v>35449830</v>
       </c>
+      <c r="F65">
+        <v>4.9629761999999999</v>
+      </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
@@ -2001,6 +2091,8 @@
       <c r="C66" t="s">
         <v>113</v>
       </c>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
@@ -2012,6 +2104,8 @@
       <c r="C67" t="s">
         <v>113</v>
       </c>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
@@ -2023,6 +2117,8 @@
       <c r="C68" t="s">
         <v>113</v>
       </c>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
@@ -2040,6 +2136,9 @@
       <c r="E69">
         <v>88591320</v>
       </c>
+      <c r="F69">
+        <v>4.4295660000000003</v>
+      </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
@@ -2057,6 +2156,9 @@
       <c r="E70">
         <v>101538599.99999999</v>
       </c>
+      <c r="F70">
+        <v>5.0769299999999999</v>
+      </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
@@ -2074,6 +2176,9 @@
       <c r="E71">
         <v>113953800</v>
       </c>
+      <c r="F71">
+        <v>5.6976899999999997</v>
+      </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
@@ -2091,6 +2196,9 @@
       <c r="E72">
         <v>2487931.034482758</v>
       </c>
+      <c r="F72">
+        <v>3.9806896549999999</v>
+      </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
@@ -2108,6 +2216,9 @@
       <c r="E73">
         <v>2596551.7241379311</v>
       </c>
+      <c r="F73">
+        <v>4.1544827590000004</v>
+      </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
@@ -2125,6 +2236,9 @@
       <c r="E74">
         <v>1582894.7368421052</v>
       </c>
+      <c r="F74">
+        <v>2.5326315789999998</v>
+      </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
@@ -2142,6 +2256,9 @@
       <c r="E75">
         <v>131246400</v>
       </c>
+      <c r="F75">
+        <v>52.498559999999998</v>
+      </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
@@ -2159,6 +2276,9 @@
       <c r="E76">
         <v>138784200</v>
       </c>
+      <c r="F76">
+        <v>55.513680000000001</v>
+      </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
@@ -2176,6 +2296,9 @@
       <c r="E77">
         <v>67396800</v>
       </c>
+      <c r="F77">
+        <v>10.10952</v>
+      </c>
       <c r="G77" s="1"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
@@ -2194,6 +2317,9 @@
       <c r="E78">
         <v>88458300</v>
       </c>
+      <c r="F78">
+        <v>13.268750000000001</v>
+      </c>
       <c r="G78" s="1"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
@@ -2212,6 +2338,9 @@
       <c r="E79">
         <v>81363900</v>
       </c>
+      <c r="F79">
+        <v>12.20459</v>
+      </c>
       <c r="G79" s="1"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
@@ -2230,8 +2359,11 @@
       <c r="E80">
         <v>73370383.333333343</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F80">
+        <v>4.4022199999999998</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>103</v>
       </c>
@@ -2247,8 +2379,11 @@
       <c r="E81">
         <v>52321200</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F81">
+        <v>3.1392699999999998</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>104</v>
       </c>
@@ -2264,8 +2399,11 @@
       <c r="E82">
         <v>106061280</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F82">
+        <v>6.3636799999999996</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>114</v>
       </c>
@@ -2281,8 +2419,11 @@
       <c r="E83">
         <v>170880</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F83">
+        <v>0.33903</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>115</v>
       </c>
@@ -2298,8 +2439,11 @@
       <c r="E84">
         <v>242560</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F84">
+        <v>0.48124</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>116</v>
       </c>
@@ -2315,8 +2459,11 @@
       <c r="E85">
         <v>277920</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F85">
+        <v>0.55139000000000005</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>117</v>
       </c>
@@ -2332,8 +2479,11 @@
       <c r="E86">
         <v>898320</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F86">
+        <v>0.56953487999999997</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>118</v>
       </c>
@@ -2349,8 +2499,11 @@
       <c r="E87">
         <v>919200</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F87">
+        <v>0.58277279999999998</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>119</v>
       </c>
@@ -2366,8 +2519,11 @@
       <c r="E88">
         <v>1054560</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F88">
+        <v>0.66859104000000003</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>120</v>
       </c>
@@ -2383,8 +2539,11 @@
       <c r="E89">
         <v>139481555.33399799</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F89">
+        <v>0.557926221</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>121</v>
       </c>
@@ -2400,8 +2559,11 @@
       <c r="E90">
         <v>142759481.03792417</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F90">
+        <v>0.57103792399999997</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>122</v>
       </c>
@@ -2417,8 +2579,11 @@
       <c r="E91">
         <v>134108178.36432715</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F91">
+        <v>0.53643271299999995</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>123</v>
       </c>
@@ -2434,8 +2599,11 @@
       <c r="E92">
         <v>26080</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F92">
+        <v>0.45029728000000002</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>124</v>
       </c>
@@ -2451,8 +2619,11 @@
       <c r="E93">
         <v>23040</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F93">
+        <v>0.39780863999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>125</v>
       </c>
@@ -2468,8 +2639,11 @@
       <c r="E94">
         <v>13440</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F94">
+        <v>0.23205503999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>126</v>
       </c>
@@ -2485,8 +2659,11 @@
       <c r="E95">
         <v>134260</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F95">
+        <v>2.75917726</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>127</v>
       </c>
@@ -2502,8 +2679,11 @@
       <c r="E96">
         <v>248920</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F96">
+        <v>5.1155549200000001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>128</v>
       </c>
@@ -2519,8 +2699,11 @@
       <c r="E97">
         <v>74560</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F97">
+        <v>1.5322825600000001</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>129</v>
       </c>
@@ -2536,8 +2719,11 @@
       <c r="E98">
         <v>169351485.14851487</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F98">
+        <v>0.169351485</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>130</v>
       </c>
@@ -2553,8 +2739,11 @@
       <c r="E99">
         <v>172402985.07462686</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F99">
+        <v>0.17240298500000001</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>131</v>
       </c>
@@ -2570,8 +2759,11 @@
       <c r="E100">
         <v>175519801.98019803</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F100">
+        <v>0.175519802</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>133</v>
       </c>
@@ -2581,8 +2773,12 @@
       <c r="C101">
         <v>116</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D101" s="2"/>
+      <c r="E101" s="3">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>134</v>
       </c>
@@ -2592,8 +2788,12 @@
       <c r="C102">
         <v>116</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D102" s="2"/>
+      <c r="E102" s="3">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>135</v>
       </c>
@@ -2603,8 +2803,12 @@
       <c r="C103">
         <v>116</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D103" s="2"/>
+      <c r="E103" s="3">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>136</v>
       </c>
@@ -2620,8 +2824,11 @@
       <c r="E104">
         <v>9145125</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F104">
+        <v>0.36580499999999999</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>137</v>
       </c>
@@ -2637,8 +2844,11 @@
       <c r="E105">
         <v>9523022.7272727285</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F105">
+        <v>0.38092090899999997</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>138</v>
       </c>
@@ -2654,8 +2864,11 @@
       <c r="E106">
         <v>7356409.0909090908</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F106">
+        <v>0.29425636399999999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>139</v>
       </c>
@@ -2671,8 +2884,11 @@
       <c r="E107">
         <v>7282845</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F107">
+        <v>0.29131000000000001</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>140</v>
       </c>
@@ -2688,8 +2904,11 @@
       <c r="E108">
         <v>8313750</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F108">
+        <v>0.33255000000000001</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>141</v>
       </c>
@@ -2705,8 +2924,11 @@
       <c r="E109">
         <v>9533100</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F109">
+        <v>0.381324</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>142</v>
       </c>
@@ -2716,8 +2938,15 @@
       <c r="C110" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D110" s="2"/>
+      <c r="E110" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="F110">
+        <v>2.6808257310632899</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>143</v>
       </c>
@@ -2727,8 +2956,15 @@
       <c r="C111" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D111" s="2"/>
+      <c r="E111" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="F111">
+        <v>2.6808257310632899</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>144</v>
       </c>
@@ -2738,8 +2974,15 @@
       <c r="C112" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D112" s="2"/>
+      <c r="E112" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="F112">
+        <v>2.6808257310632899</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>145</v>
       </c>
@@ -2749,8 +2992,15 @@
       <c r="C113" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D113" s="2"/>
+      <c r="E113" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="F113">
+        <v>0.65449846949787349</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>146</v>
       </c>
@@ -2760,8 +3010,15 @@
       <c r="C114" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D114" s="2"/>
+      <c r="E114" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="F114">
+        <v>0.65449846949787349</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>147</v>
       </c>
@@ -2771,8 +3028,15 @@
       <c r="C115" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D115" s="2"/>
+      <c r="E115" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="F115">
+        <v>0.65449846949787349</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>148</v>
       </c>
@@ -2782,8 +3046,15 @@
       <c r="C116" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D116" s="2"/>
+      <c r="E116" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="F116">
+        <v>0.33510321638291124</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>149</v>
       </c>
@@ -2793,8 +3064,15 @@
       <c r="C117" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D117" s="2"/>
+      <c r="E117" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="F117">
+        <v>0.33510321638291124</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>150</v>
       </c>
@@ -2804,8 +3082,15 @@
       <c r="C118" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D118" s="2"/>
+      <c r="E118" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="F118">
+        <v>0.33510321638291124</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>151</v>
       </c>
@@ -2815,8 +3100,12 @@
       <c r="C119" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D119" s="2"/>
+      <c r="E119" s="3">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>152</v>
       </c>
@@ -2826,8 +3115,12 @@
       <c r="C120" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D120" s="2"/>
+      <c r="E120" s="3">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>153</v>
       </c>
@@ -2837,8 +3130,12 @@
       <c r="C121" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D121" s="2"/>
+      <c r="E121" s="3">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>154</v>
       </c>
@@ -2848,8 +3145,12 @@
       <c r="C122" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D122" s="2"/>
+      <c r="E122" s="3">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>155</v>
       </c>
@@ -2859,8 +3160,12 @@
       <c r="C123" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D123" s="2"/>
+      <c r="E123" s="3">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>156</v>
       </c>
@@ -2869,6 +3174,10 @@
       </c>
       <c r="C124" t="s">
         <v>162</v>
+      </c>
+      <c r="D124" s="2"/>
+      <c r="E124" s="3">
+        <v>10000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>